<commit_message>
softwarekonzept GUI-Prototyp - Fortsetzung
</commit_message>
<xml_diff>
--- a/documents/zeitaufzeichnung/Zeitaufzeichnung-Ismail-Uener.xlsx
+++ b/documents/zeitaufzeichnung/Zeitaufzeichnung-Ismail-Uener.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\43660\OneDrive\Desktop\UIBK\UIBK\8. SEMESTER\SE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\43660\IdeaProjects\g6t1\documents\zeitaufzeichnung\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{112D7D80-BB06-4456-9D79-26684068C9BA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7DA851D-38AB-4714-A91E-C6C7A77110EB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6E71D473-8E99-584F-9CE7-0EC5B1B78532}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6E71D473-8E99-584F-9CE7-0EC5B1B78532}"/>
   </bookViews>
   <sheets>
     <sheet name="Datenerfassung" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="21">
   <si>
     <t>Datum</t>
   </si>
@@ -522,7 +522,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D7" sqref="D7"/>
+      <selection pane="bottomRight" activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6"/>
@@ -630,9 +630,18 @@
       </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="8"/>
-      <c r="B8" s="7"/>
-      <c r="D8" s="3"/>
+      <c r="A8" s="8">
+        <v>44271</v>
+      </c>
+      <c r="B8" s="7">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="8"/>

</xml_diff>

<commit_message>
GUI - Login + update Zeit
</commit_message>
<xml_diff>
--- a/documents/zeitaufzeichnung/Zeitaufzeichnung-Ismail-Uener.xlsx
+++ b/documents/zeitaufzeichnung/Zeitaufzeichnung-Ismail-Uener.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\43660\IdeaProjects\g6t1\documents\zeitaufzeichnung\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74037820-EA0B-4C7A-AA7E-A45160B1EC22}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5CD8D04-D38F-4ED0-A2B8-44696D4BEA03}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6E71D473-8E99-584F-9CE7-0EC5B1B78532}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Datenerfassung" sheetId="1" r:id="rId1"/>
     <sheet name="Tätigkeiten" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="25">
   <si>
     <t>Datum</t>
   </si>
@@ -114,6 +114,12 @@
   </si>
   <si>
     <t>AuditLogService, AuditLogRepo</t>
+  </si>
+  <si>
+    <t>UserRegistrierung</t>
+  </si>
+  <si>
+    <t>GUI</t>
   </si>
 </sst>
 </file>
@@ -528,7 +534,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D19" sqref="D19"/>
+      <selection pane="bottomRight" activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6"/>
@@ -706,39 +712,102 @@
       </c>
     </row>
     <row r="13" spans="1:4">
-      <c r="A13" s="8"/>
-      <c r="B13" s="7"/>
-      <c r="D13" s="3"/>
+      <c r="A13" s="8">
+        <v>44280</v>
+      </c>
+      <c r="B13" s="7">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="C13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="14" spans="1:4">
-      <c r="A14" s="8"/>
-      <c r="B14" s="7"/>
-      <c r="D14" s="3"/>
+      <c r="A14" s="8">
+        <v>44281</v>
+      </c>
+      <c r="B14" s="7">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="C14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="15" spans="1:4">
-      <c r="A15" s="8"/>
-      <c r="B15" s="7"/>
-      <c r="D15" s="3"/>
+      <c r="A15" s="8">
+        <v>44282</v>
+      </c>
+      <c r="B15" s="7">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="C15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="16" spans="1:4">
-      <c r="A16" s="8"/>
-      <c r="B16" s="7"/>
-      <c r="D16" s="3"/>
+      <c r="A16" s="8">
+        <v>44287</v>
+      </c>
+      <c r="B16" s="7">
+        <v>3.125E-2</v>
+      </c>
+      <c r="C16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="17" spans="1:4">
-      <c r="A17" s="8"/>
-      <c r="B17" s="7"/>
-      <c r="D17" s="3"/>
+      <c r="A17" s="8">
+        <v>44288</v>
+      </c>
+      <c r="B17" s="7">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="C17" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="18" spans="1:4">
-      <c r="A18" s="8"/>
-      <c r="B18" s="7"/>
-      <c r="D18" s="3"/>
+      <c r="A18" s="8">
+        <v>44290</v>
+      </c>
+      <c r="B18" s="7">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="C18" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="19" spans="1:4">
-      <c r="A19" s="8"/>
-      <c r="B19" s="7"/>
-      <c r="D19" s="3"/>
+      <c r="A19" s="8">
+        <v>44293</v>
+      </c>
+      <c r="B19" s="7">
+        <v>3.125E-2</v>
+      </c>
+      <c r="C19" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="8"/>

</xml_diff>

<commit_message>
GUI + update zeit
</commit_message>
<xml_diff>
--- a/documents/zeitaufzeichnung/Zeitaufzeichnung-Ismail-Uener.xlsx
+++ b/documents/zeitaufzeichnung/Zeitaufzeichnung-Ismail-Uener.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\43660\IdeaProjects\g6t1\documents\zeitaufzeichnung\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5CD8D04-D38F-4ED0-A2B8-44696D4BEA03}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33D50C35-E227-40CF-BFE8-6C1780BCB141}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6E71D473-8E99-584F-9CE7-0EC5B1B78532}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="25">
   <si>
     <t>Datum</t>
   </si>
@@ -534,7 +534,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B20" sqref="B20"/>
+      <selection pane="bottomRight" activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6"/>
@@ -810,19 +810,46 @@
       </c>
     </row>
     <row r="20" spans="1:4">
-      <c r="A20" s="8"/>
-      <c r="B20" s="7"/>
-      <c r="D20" s="3"/>
+      <c r="A20" s="8">
+        <v>44294</v>
+      </c>
+      <c r="B20" s="7">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="C20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="21" spans="1:4">
-      <c r="A21" s="8"/>
-      <c r="B21" s="7"/>
-      <c r="D21" s="3"/>
+      <c r="A21" s="8">
+        <v>44295</v>
+      </c>
+      <c r="B21" s="7">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="C21" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="22" spans="1:4">
-      <c r="A22" s="8"/>
-      <c r="B22" s="7"/>
-      <c r="D22" s="3"/>
+      <c r="A22" s="8">
+        <v>44296</v>
+      </c>
+      <c r="B22" s="7">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="C22" t="s">
+        <v>5</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="8"/>

</xml_diff>

<commit_message>
frontend categories.xhtml, create Topic with a bug, have to be fixed, extra Topic Controller (helper), bugs will be fixed
</commit_message>
<xml_diff>
--- a/documents/zeitaufzeichnung/Zeitaufzeichnung-Ismail-Uener.xlsx
+++ b/documents/zeitaufzeichnung/Zeitaufzeichnung-Ismail-Uener.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\43660\IdeaProjects\g6t1\documents\zeitaufzeichnung\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33D50C35-E227-40CF-BFE8-6C1780BCB141}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B7F9051-E2AD-4213-B810-BF7B119F1F7C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6E71D473-8E99-584F-9CE7-0EC5B1B78532}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="26">
   <si>
     <t>Datum</t>
   </si>
@@ -120,6 +120,9 @@
   </si>
   <si>
     <t>GUI</t>
+  </si>
+  <si>
+    <t>Create New Topic - categories.xhtml</t>
   </si>
 </sst>
 </file>
@@ -534,7 +537,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E22" sqref="E22"/>
+      <selection pane="bottomRight" activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6"/>
@@ -852,29 +855,74 @@
       </c>
     </row>
     <row r="23" spans="1:4">
-      <c r="A23" s="8"/>
-      <c r="B23" s="7"/>
-      <c r="D23" s="3"/>
+      <c r="A23" s="8">
+        <v>44297</v>
+      </c>
+      <c r="B23" s="7">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="C23" t="s">
+        <v>5</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="24" spans="1:4">
-      <c r="A24" s="8"/>
-      <c r="B24" s="7"/>
-      <c r="D24" s="3"/>
+      <c r="A24" s="8">
+        <v>44298</v>
+      </c>
+      <c r="B24" s="7">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="C24" t="s">
+        <v>5</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="25" spans="1:4">
-      <c r="A25" s="8"/>
-      <c r="B25" s="7"/>
-      <c r="D25" s="3"/>
+      <c r="A25" s="8">
+        <v>44300</v>
+      </c>
+      <c r="B25" s="7">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="C25" t="s">
+        <v>5</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="26" spans="1:4">
-      <c r="A26" s="8"/>
-      <c r="B26" s="7"/>
-      <c r="D26" s="3"/>
+      <c r="A26" s="8">
+        <v>44301</v>
+      </c>
+      <c r="B26" s="7">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="C26" t="s">
+        <v>5</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="27" spans="1:4">
-      <c r="A27" s="8"/>
-      <c r="B27" s="7"/>
-      <c r="D27" s="3"/>
+      <c r="A27" s="8">
+        <v>44302</v>
+      </c>
+      <c r="B27" s="7">
+        <v>0.125</v>
+      </c>
+      <c r="C27" t="s">
+        <v>5</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="8"/>

</xml_diff>